<commit_message>
Update the tasks of Know Eligibility User Story
</commit_message>
<xml_diff>
--- a/Documents/Agile-product-backlog-template.xlsx
+++ b/Documents/Agile-product-backlog-template.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="34">
   <si>
     <t xml:space="preserve">Agile Product Backlog</t>
   </si>
@@ -74,7 +74,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">The Customer will enter all personal details </t>
+      <t xml:space="preserve">Create a form to enter all personal details </t>
     </r>
     <r>
       <rPr>
@@ -84,26 +84,23 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">like Name, age, sex, dob, address, employment type, employer name, salary, emi(if any),email id, gender, purpose of loan(currently only personal loan) </t>
+      <t xml:space="preserve">like Name, age, sex, date of birth, address, employment type, employer name, salary, EMI(if any),email id, gender, purpose of loan(currently only personal loan) </t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Validate the details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The system checks the eligibility of the user through the loan eligibility calculator.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The eligible user will be displayed with the loan amount, tenure and rate of interest.</t>
+    <t xml:space="preserve">Validate the above recorded details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check the eligibility of the user using the loan eligibility calculator.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display the eligibility status to the customer. The customer is given an option to continue with the loan applcation process if eligible.</t>
   </si>
   <si>
     <t xml:space="preserve">Medium</t>
   </si>
   <si>
-    <t xml:space="preserve">The willing customer will click on upload documents button.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redirects to upload documents web page.</t>
+    <t xml:space="preserve">Redirect  to upload documents web page when clicked on ‘Upload Documents Button’.</t>
   </si>
   <si>
     <t xml:space="preserve">Sprint 2</t>
@@ -161,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -210,6 +207,11 @@
       <name val="Book Antiqua"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Book Antiqua"/>
+      <family val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -308,11 +310,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -349,19 +351,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -369,7 +371,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -452,14 +458,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>93600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>746640</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:colOff>746280</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -472,8 +478,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="11878560"/>
-          <a:ext cx="18184320" cy="4308120"/>
+          <a:off x="0" y="11689200"/>
+          <a:ext cx="18183960" cy="4308120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -493,10 +499,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC67"/>
+  <dimension ref="A1:AC1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -729,7 +735,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>10</v>
@@ -802,7 +808,7 @@
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
         <v>14</v>
       </c>
@@ -847,7 +853,7 @@
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -892,8 +898,8 @@
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+    <row r="11" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -937,8 +943,8 @@
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+    <row r="12" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -954,7 +960,7 @@
         <v>12</v>
       </c>
       <c r="F12" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>10</v>
@@ -982,26 +988,26 @@
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+    <row r="13" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="7" t="s">
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="F13" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="2"/>
@@ -1027,26 +1033,26 @@
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+    <row r="14" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="G14" s="5" t="s">
+      <c r="F14" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="H14" s="2"/>
@@ -1072,7 +1078,7 @@
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
         <v>22</v>
       </c>
@@ -1083,13 +1089,13 @@
         <v>10</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="11" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>10</v>
@@ -1117,26 +1123,26 @@
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
+    <row r="16" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="7" t="s">
+      <c r="B16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="11" t="n">
-        <v>10</v>
-      </c>
-      <c r="G16" s="7" t="s">
+      <c r="F16" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H16" s="2"/>
@@ -1162,26 +1168,26 @@
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+    <row r="17" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="B17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="F17" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>10</v>
       </c>
       <c r="H17" s="2"/>
@@ -1218,13 +1224,13 @@
         <v>10</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>10</v>
@@ -1252,26 +1258,26 @@
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
+    <row r="19" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="7" t="s">
+      <c r="B19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="G19" s="7" t="s">
+      <c r="F19" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H19" s="2"/>
@@ -1297,26 +1303,26 @@
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
+    <row r="20" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="B20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="G20" s="5" t="s">
+      <c r="F20" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>10</v>
       </c>
       <c r="H20" s="2"/>
@@ -1353,7 +1359,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>12</v>
@@ -1387,26 +1393,26 @@
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
+    <row r="22" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="7" t="s">
+      <c r="B22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="11" t="n">
+      <c r="F22" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H22" s="2"/>
@@ -1432,26 +1438,26 @@
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
+    <row r="23" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="B23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="5" t="n">
+      <c r="F23" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="7" t="s">
         <v>10</v>
       </c>
       <c r="H23" s="2"/>
@@ -1477,34 +1483,20 @@
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
+    <row r="24" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="13"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
@@ -1646,20 +1638,20 @@
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="13"/>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
@@ -2824,48 +2816,18 @@
       <c r="AB66" s="2"/>
       <c r="AC66" s="2"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
-      <c r="L67" s="2"/>
-      <c r="M67" s="2"/>
-      <c r="N67" s="2"/>
-      <c r="O67" s="2"/>
-      <c r="P67" s="2"/>
-      <c r="Q67" s="2"/>
-      <c r="R67" s="2"/>
-      <c r="S67" s="2"/>
-      <c r="T67" s="2"/>
-      <c r="U67" s="2"/>
-      <c r="V67" s="2"/>
-      <c r="W67" s="2"/>
-      <c r="X67" s="2"/>
-      <c r="Y67" s="2"/>
-      <c r="Z67" s="2"/>
-      <c r="AA67" s="2"/>
-      <c r="AB67" s="2"/>
-      <c r="AC67" s="2"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B7:C24 G7:G24" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B7:C23 G7:G23" type="list">
       <formula1>YesNo</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D7:D24" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D7:D23" type="list">
       <formula1>Priority</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E7:E24" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E7:E23" type="list">
       <formula1>Status</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2899,34 +2861,34 @@
   <sheetData>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>12</v>

</xml_diff>